<commit_message>
Add BurnDown Diagramm for Presentation (edited > new backlog)
</commit_message>
<xml_diff>
--- a/ch.bfh.bti7081.s2013.yellow/doc/cs1_task14/burndowndiag.xlsx
+++ b/ch.bfh.bti7081.s2013.yellow/doc/cs1_task14/burndowndiag.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="100" windowWidth="26120" windowHeight="24020" tabRatio="500"/>
+    <workbookView xWindow="1720" yWindow="100" windowWidth="26120" windowHeight="24020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Burndown Chart yellow</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Sprint Reviews</t>
+  </si>
+  <si>
+    <t>Gestalten der Weboberfläche, welche geöffnet wird beim Klick auf den Link in der Notification zur Bestätigung der Einnahme.</t>
+  </si>
+  <si>
+    <t>Übersichtseite für Arzt mit  Prescriptions mit Sortier- und Filterfunktion.</t>
   </si>
 </sst>
 </file>
@@ -252,7 +258,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -306,6 +312,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -350,7 +362,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blatt1!$A$19</c:f>
+              <c:f>Blatt1!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -402,39 +414,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blatt1!$C$19:$L$19</c:f>
+              <c:f>Blatt1!$C$21:$L$21</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>97.0</c:v>
+                  <c:v>113.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>86.22222222222223</c:v>
+                  <c:v>100.4444444444444</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75.44444444444445</c:v>
+                  <c:v>87.88888888888889</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>64.66666666666668</c:v>
+                  <c:v>75.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53.88888888888891</c:v>
+                  <c:v>62.77777777777777</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43.11111111111113</c:v>
+                  <c:v>50.22222222222221</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32.33333333333335</c:v>
+                  <c:v>37.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.55555555555557</c:v>
+                  <c:v>25.1111111111111</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.77777777777779</c:v>
+                  <c:v>12.55555555555554</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.4210854715202E-14</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -446,7 +458,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blatt1!$A$20</c:f>
+              <c:f>Blatt1!$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -504,36 +516,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blatt1!$C$20:$L$20</c:f>
+              <c:f>Blatt1!$C$22:$L$22</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>90.0</c:v>
+                  <c:v>109.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80.0</c:v>
+                  <c:v>97.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.0</c:v>
+                  <c:v>85.16666666666665</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60.0</c:v>
+                  <c:v>72.99999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>60.83333333333332</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40.0</c:v>
+                  <c:v>48.66666666666666</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.0</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.0</c:v>
+                  <c:v>24.33333333333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.0</c:v>
+                  <c:v>12.16666666666666</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.0</c:v>
@@ -548,7 +560,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Blatt1!$A$21</c:f>
+              <c:f>Blatt1!$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -606,33 +618,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Blatt1!$C$21:$L$21</c:f>
+              <c:f>Blatt1!$C$23:$L$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>90.0</c:v>
+                  <c:v>109.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.0</c:v>
+                  <c:v>96.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74.0</c:v>
+                  <c:v>92.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>62.0</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47.5</c:v>
+                  <c:v>54.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.5</c:v>
+                  <c:v>40.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.5</c:v>
+                  <c:v>23.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>5.0</c:v>
@@ -655,11 +667,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2074413208"/>
-        <c:axId val="2073198552"/>
+        <c:axId val="2074424440"/>
+        <c:axId val="2076955576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2074413208"/>
+        <c:axId val="2074424440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -668,7 +680,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073198552"/>
+        <c:crossAx val="2076955576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -676,7 +688,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2073198552"/>
+        <c:axId val="2076955576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -687,7 +699,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074413208"/>
+        <c:crossAx val="2074424440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -715,13 +727,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1066,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1191,7 +1203,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="17">
-        <f t="shared" ref="C5:C18" si="0">SUM(D5:L5)</f>
+        <f t="shared" ref="C5:C20" si="0">SUM(D5:L5)</f>
         <v>7</v>
       </c>
       <c r="D5" s="21">
@@ -1220,13 +1232,13 @@
       </c>
       <c r="C6" s="17">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" s="21">
         <v>4</v>
       </c>
       <c r="E6" s="21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
@@ -1286,83 +1298,87 @@
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" ht="30">
-      <c r="A9" s="10" t="s">
-        <v>16</v>
+      <c r="A9" s="23" t="s">
+        <v>35</v>
       </c>
       <c r="B9" s="15">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="17">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21">
+        <f>SUM(D9:L9)</f>
+        <v>15</v>
+      </c>
+      <c r="D9" s="21">
         <v>1</v>
       </c>
+      <c r="E9" s="21">
+        <v>2</v>
+      </c>
+      <c r="F9" s="21">
+        <v>6</v>
+      </c>
+      <c r="G9" s="21">
+        <v>4</v>
+      </c>
+      <c r="H9" s="21"/>
       <c r="I9" s="21">
-        <v>4</v>
-      </c>
-      <c r="J9" s="21">
         <v>2</v>
       </c>
+      <c r="J9" s="21"/>
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" ht="45">
+    <row r="10" spans="1:13" ht="30">
       <c r="A10" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="15">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C10" s="17">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H10" s="21">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I10" s="21">
-        <v>4</v>
-      </c>
-      <c r="J10" s="21"/>
+        <v>6</v>
+      </c>
+      <c r="J10" s="21">
+        <v>2</v>
+      </c>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" ht="45">
       <c r="A11" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="15">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C11" s="17">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
-      <c r="G11" s="21">
-        <v>5</v>
-      </c>
+      <c r="G11" s="21"/>
       <c r="H11" s="21">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I11" s="21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J11" s="21"/>
       <c r="K11" s="21"/>
@@ -1371,48 +1387,48 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="15">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C12" s="17">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>SUM(D12:L12)</f>
+        <v>0</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
-      <c r="H12" s="21">
-        <v>6</v>
-      </c>
-      <c r="I12" s="21">
-        <v>2</v>
-      </c>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
       <c r="J12" s="21"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
       <c r="M12" s="2"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="16">
-        <v>4</v>
+      <c r="A13" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="15">
+        <v>8</v>
       </c>
       <c r="C13" s="17">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>SUM(D13:L13)</f>
+        <v>7</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
+      <c r="G13" s="21">
+        <v>5</v>
+      </c>
+      <c r="H13" s="21">
+        <v>1</v>
+      </c>
       <c r="I13" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J13" s="21"/>
       <c r="K13" s="21"/>
@@ -1421,88 +1437,88 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" s="15">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C14" s="17">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21">
+      <c r="H14" s="21">
         <v>6</v>
       </c>
+      <c r="I14" s="21">
+        <v>2</v>
+      </c>
+      <c r="J14" s="21"/>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
       <c r="M14" s="2"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" s="16">
         <v>4</v>
       </c>
       <c r="C15" s="17">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>2</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21">
-        <v>2.5</v>
-      </c>
-      <c r="K15" s="21">
+      <c r="I15" s="21">
         <v>2</v>
       </c>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
       <c r="L15" s="21"/>
       <c r="M15" s="2"/>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" s="15">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C16" s="17">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>6</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
-      <c r="G16" s="21">
-        <v>1.5</v>
-      </c>
+      <c r="G16" s="21"/>
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
+      <c r="J16" s="21">
+        <v>6</v>
+      </c>
       <c r="K16" s="21"/>
       <c r="L16" s="21"/>
       <c r="M16" s="2"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="15">
+      <c r="A17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="16">
         <v>4</v>
       </c>
       <c r="C17" s="17">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
@@ -1510,183 +1526,235 @@
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
+      <c r="J17" s="21">
+        <v>2.5</v>
+      </c>
       <c r="K17" s="21">
         <v>2</v>
       </c>
-      <c r="L17" s="21">
-        <v>2</v>
-      </c>
+      <c r="L17" s="21"/>
       <c r="M17" s="2"/>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B18" s="15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" s="17">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
-      <c r="F18" s="21">
-        <v>1</v>
-      </c>
-      <c r="G18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21">
+        <v>2</v>
+      </c>
       <c r="H18" s="21"/>
-      <c r="I18" s="21">
-        <v>0.5</v>
-      </c>
+      <c r="I18" s="21"/>
       <c r="J18" s="21"/>
-      <c r="K18" s="21">
-        <v>1.5</v>
-      </c>
+      <c r="K18" s="21"/>
       <c r="L18" s="21"/>
       <c r="M18" s="2"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="15">
+        <v>4</v>
+      </c>
+      <c r="C19" s="17">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21">
+        <v>2</v>
+      </c>
+      <c r="K19" s="21">
+        <v>4</v>
+      </c>
+      <c r="L19" s="21">
+        <v>2</v>
+      </c>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="15">
+        <v>3</v>
+      </c>
+      <c r="C20" s="17">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21">
+        <v>1</v>
+      </c>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21">
+        <v>1.5</v>
+      </c>
+      <c r="L20" s="21"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="22">
-        <f>SUM(B4:B18)</f>
-        <v>97</v>
-      </c>
-      <c r="D19" s="12">
-        <f>C19-$C$19/9</f>
-        <v>86.222222222222229</v>
-      </c>
-      <c r="E19" s="12">
-        <f>D19-$C$19/9</f>
-        <v>75.444444444444457</v>
-      </c>
-      <c r="F19" s="12">
-        <f t="shared" ref="F19:L19" si="1">E19-$C$19/9</f>
-        <v>64.666666666666686</v>
-      </c>
-      <c r="G19" s="12">
+      <c r="B21" s="16"/>
+      <c r="C21" s="22">
+        <f>SUM(B4:B20)</f>
+        <v>113</v>
+      </c>
+      <c r="D21" s="12">
+        <f>C21-$C$21/9</f>
+        <v>100.44444444444444</v>
+      </c>
+      <c r="E21" s="12">
+        <f>D21-$C$21/9</f>
+        <v>87.888888888888886</v>
+      </c>
+      <c r="F21" s="12">
+        <f t="shared" ref="F21:L21" si="1">E21-$C$21/9</f>
+        <v>75.333333333333329</v>
+      </c>
+      <c r="G21" s="12">
         <f t="shared" si="1"/>
-        <v>53.888888888888907</v>
-      </c>
-      <c r="H19" s="12">
+        <v>62.777777777777771</v>
+      </c>
+      <c r="H21" s="12">
         <f t="shared" si="1"/>
-        <v>43.111111111111128</v>
-      </c>
-      <c r="I19" s="12">
+        <v>50.222222222222214</v>
+      </c>
+      <c r="I21" s="12">
         <f t="shared" si="1"/>
-        <v>32.33333333333335</v>
-      </c>
-      <c r="J19" s="12">
+        <v>37.666666666666657</v>
+      </c>
+      <c r="J21" s="12">
         <f t="shared" si="1"/>
-        <v>21.555555555555571</v>
-      </c>
-      <c r="K19" s="12">
+        <v>25.1111111111111</v>
+      </c>
+      <c r="K21" s="12">
         <f t="shared" si="1"/>
-        <v>10.777777777777793</v>
-      </c>
-      <c r="L19" s="12">
+        <v>12.555555555555545</v>
+      </c>
+      <c r="L21" s="12">
         <f t="shared" si="1"/>
-        <v>1.4210854715202004E-14</v>
-      </c>
-      <c r="M19" s="7"/>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M21" s="7"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="17">
-        <f>SUM(C4:C18)</f>
-        <v>90</v>
-      </c>
-      <c r="D20" s="18">
-        <f>C20-$C$20/9</f>
-        <v>80</v>
-      </c>
-      <c r="E20" s="18">
-        <f t="shared" ref="E20:L20" si="2">D20-$C$20/9</f>
-        <v>70</v>
-      </c>
-      <c r="F20" s="18">
+      <c r="B22" s="13"/>
+      <c r="C22" s="17">
+        <f>SUM(C4:C20)</f>
+        <v>109.5</v>
+      </c>
+      <c r="D22" s="18">
+        <f>C22-$C$22/9</f>
+        <v>97.333333333333329</v>
+      </c>
+      <c r="E22" s="18">
+        <f t="shared" ref="E22:L22" si="2">D22-$C$22/9</f>
+        <v>85.166666666666657</v>
+      </c>
+      <c r="F22" s="18">
         <f t="shared" si="2"/>
-        <v>60</v>
-      </c>
-      <c r="G20" s="18">
+        <v>72.999999999999986</v>
+      </c>
+      <c r="G22" s="18">
         <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="H20" s="18">
+        <v>60.833333333333321</v>
+      </c>
+      <c r="H22" s="18">
         <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="I20" s="18">
+        <v>48.666666666666657</v>
+      </c>
+      <c r="I22" s="18">
         <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="J20" s="18">
+        <v>36.499999999999993</v>
+      </c>
+      <c r="J22" s="18">
         <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="K20" s="18">
+        <v>24.333333333333329</v>
+      </c>
+      <c r="K22" s="18">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="L20" s="18">
+        <v>12.166666666666663</v>
+      </c>
+      <c r="L22" s="18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M20" s="7"/>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="20" t="s">
+      <c r="M22" s="7"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14">
-        <f>C20</f>
-        <v>90</v>
-      </c>
-      <c r="D21" s="14">
-        <f>C20-SUM(D4:D17)</f>
-        <v>78</v>
-      </c>
-      <c r="E21" s="14">
-        <f>D21-SUM(E4:E17)</f>
-        <v>74</v>
-      </c>
-      <c r="F21" s="14">
-        <f t="shared" ref="F21:L21" si="3">E21-SUM(F4:F17)</f>
-        <v>62</v>
-      </c>
-      <c r="G21" s="14">
+      <c r="B23" s="14"/>
+      <c r="C23" s="14">
+        <f>C22</f>
+        <v>109.5</v>
+      </c>
+      <c r="D23" s="14">
+        <f>C22-SUM(D4:D19)</f>
+        <v>96.5</v>
+      </c>
+      <c r="E23" s="14">
+        <f>D23-SUM(E4:E19)</f>
+        <v>92.5</v>
+      </c>
+      <c r="F23" s="14">
+        <f t="shared" ref="F23:L23" si="3">E23-SUM(F4:F19)</f>
+        <v>74.5</v>
+      </c>
+      <c r="G23" s="14">
         <f t="shared" si="3"/>
-        <v>47.5</v>
-      </c>
-      <c r="H21" s="14">
+        <v>54.5</v>
+      </c>
+      <c r="H23" s="14">
         <f t="shared" si="3"/>
-        <v>32.5</v>
-      </c>
-      <c r="I21" s="14">
+        <v>40.5</v>
+      </c>
+      <c r="I23" s="14">
         <f t="shared" si="3"/>
-        <v>19.5</v>
-      </c>
-      <c r="J21" s="14">
+        <v>23.5</v>
+      </c>
+      <c r="J23" s="14">
         <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="K21" s="14">
+        <v>11</v>
+      </c>
+      <c r="K23" s="14">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="L21" s="14">
+      <c r="L23" s="14">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="M21" s="7"/>
+      <c r="M23" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>